<commit_message>
Tabajando con reportes DHL
</commit_message>
<xml_diff>
--- a/BusiNext/Clientes/new_reports/clientes_prospecto_web.xlsx
+++ b/BusiNext/Clientes/new_reports/clientes_prospecto_web.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="444">
   <si>
     <t>username</t>
   </si>
@@ -31,6 +31,21 @@
     <t>&lt;NULL&gt;</t>
   </si>
   <si>
+    <t>olga</t>
+  </si>
+  <si>
+    <t>Rebecabc</t>
+  </si>
+  <si>
+    <t>Vang</t>
+  </si>
+  <si>
+    <t>RefGamboa</t>
+  </si>
+  <si>
+    <t>HugoCaloca</t>
+  </si>
+  <si>
     <t>Doriss</t>
   </si>
   <si>
@@ -40,15 +55,33 @@
     <t>Cris</t>
   </si>
   <si>
+    <t>99E1MLLKJX</t>
+  </si>
+  <si>
+    <t>BYOVDDF5BU</t>
+  </si>
+  <si>
+    <t>SZSXAO3XOW</t>
+  </si>
+  <si>
     <t>Jose</t>
   </si>
   <si>
+    <t>REPMF6ILIQ</t>
+  </si>
+  <si>
     <t>Arroyo60</t>
   </si>
   <si>
     <t>yblando</t>
   </si>
   <si>
+    <t>Pauornelas</t>
+  </si>
+  <si>
+    <t>EM0C4DVVCI</t>
+  </si>
+  <si>
     <t>Zwidy</t>
   </si>
   <si>
@@ -64,6 +97,15 @@
     <t>RoeL</t>
   </si>
   <si>
+    <t>CGR8CO8J0H</t>
+  </si>
+  <si>
+    <t>8N7UVFUPEV</t>
+  </si>
+  <si>
+    <t>7RBIZ1OA95</t>
+  </si>
+  <si>
     <t>Annfzg</t>
   </si>
   <si>
@@ -103,9 +145,15 @@
     <t>Luz1802</t>
   </si>
   <si>
+    <t>camino</t>
+  </si>
+  <si>
     <t>ANA</t>
   </si>
   <si>
+    <t>Ruth1</t>
+  </si>
+  <si>
     <t>Citlalli</t>
   </si>
   <si>
@@ -115,6 +163,9 @@
     <t>Adriana20</t>
   </si>
   <si>
+    <t>W9FOLIFLKL</t>
+  </si>
+  <si>
     <t>Citlally</t>
   </si>
   <si>
@@ -136,12 +187,24 @@
     <t>Roscha</t>
   </si>
   <si>
+    <t>5P4ZLUVM88</t>
+  </si>
+  <si>
+    <t>3AHI6AXO5R</t>
+  </si>
+  <si>
+    <t>GAA1PLCUWW</t>
+  </si>
+  <si>
     <t>Erandi</t>
   </si>
   <si>
     <t>carsystems</t>
   </si>
   <si>
+    <t>XPG4VY737I</t>
+  </si>
+  <si>
     <t>_.mbac._</t>
   </si>
   <si>
@@ -157,9 +220,18 @@
     <t>100978</t>
   </si>
   <si>
+    <t>M11V4DY37D</t>
+  </si>
+  <si>
+    <t>2VUIFWLOC4</t>
+  </si>
+  <si>
     <t>Sandy</t>
   </si>
   <si>
+    <t>9WW4M1556Q</t>
+  </si>
+  <si>
     <t>CarlosVelez</t>
   </si>
   <si>
@@ -178,6 +250,9 @@
     <t>Sthefany</t>
   </si>
   <si>
+    <t>DK9V4218QY</t>
+  </si>
+  <si>
     <t>lborges</t>
   </si>
   <si>
@@ -193,6 +268,9 @@
     <t>luis83</t>
   </si>
   <si>
+    <t>Anahiramirez</t>
+  </si>
+  <si>
     <t>pancho</t>
   </si>
   <si>
@@ -217,6 +295,15 @@
     <t>aaa</t>
   </si>
   <si>
+    <t>Kenia</t>
+  </si>
+  <si>
+    <t>4EGD0JZSTD</t>
+  </si>
+  <si>
+    <t>lore</t>
+  </si>
+  <si>
     <t>LalitoJarquin</t>
   </si>
   <si>
@@ -226,12 +313,21 @@
     <t>Hermilo</t>
   </si>
   <si>
+    <t>9WCXNI11AS</t>
+  </si>
+  <si>
+    <t>ILQCC4F3PX</t>
+  </si>
+  <si>
     <t>aguilarandrea</t>
   </si>
   <si>
     <t>Leonardo</t>
   </si>
   <si>
+    <t>JoelPerez</t>
+  </si>
+  <si>
     <t>MALENNY</t>
   </si>
   <si>
@@ -250,6 +346,9 @@
     <t>JulioM</t>
   </si>
   <si>
+    <t>Mildred</t>
+  </si>
+  <si>
     <t>Checolevi</t>
   </si>
   <si>
@@ -268,9 +367,15 @@
     <t>Joel</t>
   </si>
   <si>
+    <t>QLWXP5MEB2</t>
+  </si>
+  <si>
     <t>chaparrita</t>
   </si>
   <si>
+    <t>UXVEOAOMM3</t>
+  </si>
+  <si>
     <t>4428351277</t>
   </si>
   <si>
@@ -292,9 +397,6 @@
     <t>Edy</t>
   </si>
   <si>
-    <t>CDELAB</t>
-  </si>
-  <si>
     <t>bronik</t>
   </si>
   <si>
@@ -325,6 +427,9 @@
     <t>Yuli</t>
   </si>
   <si>
+    <t>FJYV05H7LP</t>
+  </si>
+  <si>
     <t>Nani</t>
   </si>
   <si>
@@ -349,21 +454,63 @@
     <t>YRAM17</t>
   </si>
   <si>
+    <t>N8834AV8QY</t>
+  </si>
+  <si>
     <t>Runelvis</t>
   </si>
   <si>
     <t>RoseCc</t>
   </si>
   <si>
+    <t>T1ZLWBQO03</t>
+  </si>
+  <si>
     <t>Diego-kun</t>
   </si>
   <si>
+    <t>W8GYQLJKFS</t>
+  </si>
+  <si>
     <t>lopita</t>
   </si>
   <si>
+    <t>B3AJT0SWM7</t>
+  </si>
+  <si>
+    <t>Silveria</t>
+  </si>
+  <si>
+    <t>Gabita</t>
+  </si>
+  <si>
+    <t>Blanca1</t>
+  </si>
+  <si>
+    <t>marlu</t>
+  </si>
+  <si>
+    <t>ethsson</t>
+  </si>
+  <si>
+    <t>olgagarciamiranda@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rebecabc28@gmail.com </t>
+  </si>
+  <si>
     <t>rousdani_nai@hotmail.com</t>
   </si>
   <si>
+    <t>ivan.g.palacios@xtrovi.com</t>
+  </si>
+  <si>
+    <t>Refgamboa.12@gmail.com</t>
+  </si>
+  <si>
+    <t>hugocaloca@hotmail.com</t>
+  </si>
+  <si>
     <t>emi1993.yo@gmail.com</t>
   </si>
   <si>
@@ -373,15 +520,33 @@
     <t>p.amella.ste.88@gmail.com</t>
   </si>
   <si>
+    <t>Bdjxbe@bduxbe.com</t>
+  </si>
+  <si>
+    <t>Hxuen@jrick.com</t>
+  </si>
+  <si>
+    <t>Bfbej@hdjc.com</t>
+  </si>
+  <si>
     <t>elegidodzion@gmail.com</t>
   </si>
   <si>
+    <t>czsx@zxscvs.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">luz brillante.60@gmail.com </t>
   </si>
   <si>
     <t>yblando.yb@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Paulletornelas@gmail.com </t>
+  </si>
+  <si>
+    <t>vfvdfv@dsca.com</t>
+  </si>
+  <si>
     <t>zwidy2709@icloud.com</t>
   </si>
   <si>
@@ -397,6 +562,15 @@
     <t>roelvillela2002@gmail.com</t>
   </si>
   <si>
+    <t>gipalac@yahoo.com</t>
+  </si>
+  <si>
+    <t>fvdf@nkjv.com</t>
+  </si>
+  <si>
+    <t>gipalac@gmail.com</t>
+  </si>
+  <si>
     <t>anafre.182@hotmail.com</t>
   </si>
   <si>
@@ -433,15 +607,24 @@
     <t>bluz0218@gmail.com</t>
   </si>
   <si>
+    <t>caminolejos@aqui.com</t>
+  </si>
+  <si>
     <t>valeria37@hotmail.com</t>
   </si>
   <si>
+    <t>luzbrillante.60@gmail.com</t>
+  </si>
+  <si>
     <t>citlallifranco29531@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">natylara0321@gmail.com </t>
   </si>
   <si>
+    <t>miky1706@hotmail.com</t>
+  </si>
+  <si>
     <t>Citlallypadilla@yahoo.com.mx</t>
   </si>
   <si>
@@ -463,6 +646,9 @@
     <t xml:space="preserve">cinthyachava26@hotmail.com </t>
   </si>
   <si>
+    <t>Riverosalvador64@gmail.com</t>
+  </si>
+  <si>
     <t>erandi5153@gmail.com</t>
   </si>
   <si>
@@ -484,9 +670,18 @@
     <t>Lilixroy@hotmail.com</t>
   </si>
   <si>
+    <t>correo@gmail.com</t>
+  </si>
+  <si>
+    <t>gabrielperezgonzalez702@gmail.com</t>
+  </si>
+  <si>
     <t>sandy_minidi@hotmail.com</t>
   </si>
   <si>
+    <t>leonardosr_99@outlook.com</t>
+  </si>
+  <si>
     <t>carloseduardovelezflores@gmail.com</t>
   </si>
   <si>
@@ -502,6 +697,9 @@
     <t xml:space="preserve">maribelvaldezvarela6@gmail.com </t>
   </si>
   <si>
+    <t>breencasarrubias27@gmail.com</t>
+  </si>
+  <si>
     <t>lisvethborges711@gmail.com</t>
   </si>
   <si>
@@ -517,6 +715,9 @@
     <t>nerigordillo94@gmail.com</t>
   </si>
   <si>
+    <t>hildaramirezvalerio@gmail.com</t>
+  </si>
+  <si>
     <t>fhksbewkwj@gmail.com</t>
   </si>
   <si>
@@ -541,18 +742,36 @@
     <t>aaa@fke-mail.aaa</t>
   </si>
   <si>
+    <t>Kenia_030408@hotmail.com</t>
+  </si>
+  <si>
+    <t>analuher.2401@gmail.com</t>
+  </si>
+  <si>
+    <t>lorena692@gmail.com</t>
+  </si>
+  <si>
     <t>eduardo_jarquin87@outlook.com</t>
   </si>
   <si>
     <t>Naomijazmin0@gmail.com</t>
   </si>
   <si>
+    <t>jorgenegrete524@gmail.com</t>
+  </si>
+  <si>
+    <t>gipalacs@gmail.con</t>
+  </si>
+  <si>
     <t>batistae@gmail.com</t>
   </si>
   <si>
     <t>leojpc98@gmail.com</t>
   </si>
   <si>
+    <t>angeleschairez@yahoo.com.mx</t>
+  </si>
+  <si>
     <t>malennyjaimes33@gmail.com</t>
   </si>
   <si>
@@ -571,6 +790,9 @@
     <t>jmoncada.haaz@yahoo.com.mx</t>
   </si>
   <si>
+    <t>gema.mildred09@gmail.com</t>
+  </si>
+  <si>
     <t>checo.levi09@gmail.com</t>
   </si>
   <si>
@@ -589,9 +811,15 @@
     <t>tijerineitor@gmail.com</t>
   </si>
   <si>
+    <t>elisarrios1@hotmail.com</t>
+  </si>
+  <si>
     <t>noraavila@ymail.com</t>
   </si>
   <si>
+    <t>ja23@gmail.com</t>
+  </si>
+  <si>
     <t>jsantillan.topclean@gmail.com</t>
   </si>
   <si>
@@ -613,9 +841,6 @@
     <t>tovar764@gmail.com</t>
   </si>
   <si>
-    <t>leon_axa_carlos@hotmail.com</t>
-  </si>
-  <si>
     <t>alvaortzveronica@gmail.com</t>
   </si>
   <si>
@@ -646,6 +871,9 @@
     <t>yulianna_rr@hotmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">mayterosalessanchez@gmail.com </t>
+  </si>
+  <si>
     <t>amjs10@hotmail.com</t>
   </si>
   <si>
@@ -670,21 +898,69 @@
     <t xml:space="preserve">Yramdeandas@gmail.com </t>
   </si>
   <si>
+    <t>bj141232@gmail.com</t>
+  </si>
+  <si>
     <t>Runelvismoreno50@mgail.com</t>
   </si>
   <si>
     <t>rrccjjaa@gmail.com</t>
   </si>
   <si>
+    <t>bdjjf@juf.com</t>
+  </si>
+  <si>
     <t>melgoza.escolar@gmail.com</t>
   </si>
   <si>
+    <t>bdjdu@neid.id</t>
+  </si>
+  <si>
     <t>lopitaymanolo29@gmail.com</t>
   </si>
   <si>
+    <t>disenotoriz@hotmail.com</t>
+  </si>
+  <si>
+    <t>silveriaurbina946@gmail.com</t>
+  </si>
+  <si>
+    <t>mendoza_gabriela@hotmail.com</t>
+  </si>
+  <si>
+    <t>blancakbk@hotmail.com</t>
+  </si>
+  <si>
+    <t>hhapi@hotmail.com</t>
+  </si>
+  <si>
+    <t>fonsecaethsson@gmail.com</t>
+  </si>
+  <si>
+    <t>7148293456</t>
+  </si>
+  <si>
+    <t>7458961245</t>
+  </si>
+  <si>
+    <t>1542367800</t>
+  </si>
+  <si>
+    <t>9841975552</t>
+  </si>
+  <si>
     <t>5574157934</t>
   </si>
   <si>
+    <t>5512232555</t>
+  </si>
+  <si>
+    <t>6567028360</t>
+  </si>
+  <si>
+    <t>5519764468</t>
+  </si>
+  <si>
     <t>7291075198</t>
   </si>
   <si>
@@ -700,6 +976,9 @@
     <t>5540722989</t>
   </si>
   <si>
+    <t>4641880935</t>
+  </si>
+  <si>
     <t>8332344604</t>
   </si>
   <si>
@@ -712,6 +991,12 @@
     <t>6321121335</t>
   </si>
   <si>
+    <t>5528985700</t>
+  </si>
+  <si>
+    <t>5528985555</t>
+  </si>
+  <si>
     <t>5548595561</t>
   </si>
   <si>
@@ -754,12 +1039,18 @@
     <t>3313960997</t>
   </si>
   <si>
+    <t>5525054503</t>
+  </si>
+  <si>
     <t>3321999377</t>
   </si>
   <si>
     <t>5581763609</t>
   </si>
   <si>
+    <t>5551844185</t>
+  </si>
+  <si>
     <t>9982307156</t>
   </si>
   <si>
@@ -781,9 +1072,21 @@
     <t>5573704224</t>
   </si>
   <si>
+    <t>6611465948</t>
+  </si>
+  <si>
+    <t>5529282222</t>
+  </si>
+  <si>
+    <t>5529282221</t>
+  </si>
+  <si>
     <t>3316025662</t>
   </si>
   <si>
+    <t>3751134157</t>
+  </si>
+  <si>
     <t>3751049107</t>
   </si>
   <si>
@@ -799,9 +1102,18 @@
     <t>5516496042</t>
   </si>
   <si>
+    <t>6671839847</t>
+  </si>
+  <si>
+    <t>2222559179</t>
+  </si>
+  <si>
     <t>5539190061</t>
   </si>
   <si>
+    <t>3315376465</t>
+  </si>
+  <si>
     <t>5587035624</t>
   </si>
   <si>
@@ -814,6 +1126,9 @@
     <t>2211039678</t>
   </si>
   <si>
+    <t>5561489455</t>
+  </si>
+  <si>
     <t>5579240457</t>
   </si>
   <si>
@@ -826,6 +1141,9 @@
     <t>4431924780</t>
   </si>
   <si>
+    <t>8661151069</t>
+  </si>
+  <si>
     <t>5581763601</t>
   </si>
   <si>
@@ -838,6 +1156,15 @@
     <t>7265001140</t>
   </si>
   <si>
+    <t>6647780203</t>
+  </si>
+  <si>
+    <t>5568608585</t>
+  </si>
+  <si>
+    <t>2251089327</t>
+  </si>
+  <si>
     <t>9515848573</t>
   </si>
   <si>
@@ -847,12 +1174,21 @@
     <t>2226080252</t>
   </si>
   <si>
+    <t>5548372765</t>
+  </si>
+  <si>
+    <t>5528980001</t>
+  </si>
+  <si>
     <t>9611755040</t>
   </si>
   <si>
     <t>4925837017</t>
   </si>
   <si>
+    <t>4921033379</t>
+  </si>
+  <si>
     <t>7551367959</t>
   </si>
   <si>
@@ -871,6 +1207,9 @@
     <t>4445149475</t>
   </si>
   <si>
+    <t>5615165471</t>
+  </si>
+  <si>
     <t>8662069662</t>
   </si>
   <si>
@@ -889,9 +1228,15 @@
     <t>3521203625</t>
   </si>
   <si>
+    <t>2281946733</t>
+  </si>
+  <si>
     <t>4381077140</t>
   </si>
   <si>
+    <t>5598714638</t>
+  </si>
+  <si>
     <t>3313398566</t>
   </si>
   <si>
@@ -910,9 +1255,6 @@
     <t>5529437043</t>
   </si>
   <si>
-    <t>5555091755</t>
-  </si>
-  <si>
     <t>2941100195</t>
   </si>
   <si>
@@ -943,6 +1285,9 @@
     <t>6252839428</t>
   </si>
   <si>
+    <t>7292655573</t>
+  </si>
+  <si>
     <t>6319996395</t>
   </si>
   <si>
@@ -964,13 +1309,40 @@
     <t>8341023266</t>
   </si>
   <si>
+    <t>5624459217</t>
+  </si>
+  <si>
     <t>3521127429</t>
   </si>
   <si>
+    <t>5529287766</t>
+  </si>
+  <si>
     <t>4428500015</t>
   </si>
   <si>
+    <t>5529388473</t>
+  </si>
+  <si>
     <t>5579251690</t>
+  </si>
+  <si>
+    <t>5530315756</t>
+  </si>
+  <si>
+    <t>5565181594</t>
+  </si>
+  <si>
+    <t>5568174493</t>
+  </si>
+  <si>
+    <t>6371133390</t>
+  </si>
+  <si>
+    <t>3521209183</t>
+  </si>
+  <si>
+    <t>5561323566</t>
   </si>
   <si>
     <t>CDMX</t>
@@ -1331,7 +1703,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1356,49 +1728,43 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>222</v>
+        <v>307</v>
       </c>
       <c r="D2" t="s">
-        <v>319</v>
+        <v>443</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>308</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>443</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>224</v>
+        <v>309</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>443</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>159</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1409,13 +1775,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>160</v>
       </c>
       <c r="C6" t="s">
-        <v>225</v>
+        <v>310</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -1423,27 +1789,27 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
-        <v>226</v>
+        <v>311</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>443</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>162</v>
       </c>
       <c r="C8" t="s">
-        <v>227</v>
+        <v>312</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -1451,13 +1817,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>163</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>313</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -1465,13 +1831,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>164</v>
       </c>
       <c r="C10" t="s">
-        <v>228</v>
+        <v>314</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -1479,13 +1845,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>165</v>
       </c>
       <c r="C11" t="s">
-        <v>229</v>
+        <v>315</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
@@ -1493,13 +1859,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
       <c r="C12" t="s">
-        <v>230</v>
+        <v>316</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
@@ -1507,13 +1873,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>167</v>
       </c>
       <c r="C13" t="s">
-        <v>231</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
@@ -1521,13 +1887,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>168</v>
       </c>
       <c r="C14" t="s">
-        <v>232</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
@@ -1535,13 +1901,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>169</v>
       </c>
       <c r="C15" t="s">
-        <v>233</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -1549,13 +1915,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>129</v>
+        <v>170</v>
       </c>
       <c r="C16" t="s">
-        <v>234</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
@@ -1563,27 +1929,27 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>171</v>
       </c>
       <c r="C17" t="s">
-        <v>235</v>
+        <v>317</v>
       </c>
       <c r="D17" t="s">
-        <v>319</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>130</v>
+        <v>172</v>
       </c>
       <c r="C18" t="s">
-        <v>236</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
@@ -1591,13 +1957,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="C19" t="s">
-        <v>237</v>
+        <v>318</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -1605,13 +1971,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>132</v>
+        <v>174</v>
       </c>
       <c r="C20" t="s">
-        <v>238</v>
+        <v>319</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
@@ -1619,13 +1985,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>133</v>
+        <v>175</v>
       </c>
       <c r="C21" t="s">
-        <v>239</v>
+        <v>320</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
@@ -1633,13 +1999,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>134</v>
+        <v>176</v>
       </c>
       <c r="C22" t="s">
-        <v>240</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
@@ -1647,13 +2013,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="C23" t="s">
-        <v>241</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
@@ -1661,13 +2027,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>136</v>
+        <v>178</v>
       </c>
       <c r="C24" t="s">
-        <v>242</v>
+        <v>321</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
@@ -1675,13 +2041,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>137</v>
+        <v>179</v>
       </c>
       <c r="C25" t="s">
-        <v>243</v>
+        <v>322</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
@@ -1689,13 +2055,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>138</v>
+        <v>180</v>
       </c>
       <c r="C26" t="s">
-        <v>244</v>
+        <v>323</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
@@ -1703,13 +2069,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="C27" t="s">
-        <v>245</v>
+        <v>324</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
@@ -1717,13 +2083,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>140</v>
+        <v>182</v>
       </c>
       <c r="C28" t="s">
-        <v>246</v>
+        <v>325</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
@@ -1731,13 +2097,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>183</v>
       </c>
       <c r="C29" t="s">
-        <v>247</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
@@ -1745,13 +2111,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>141</v>
+        <v>184</v>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
+        <v>326</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
@@ -1759,13 +2125,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>142</v>
+        <v>185</v>
       </c>
       <c r="C31" t="s">
-        <v>248</v>
+        <v>327</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
@@ -1773,13 +2139,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>143</v>
+        <v>186</v>
       </c>
       <c r="C32" t="s">
-        <v>249</v>
+        <v>328</v>
       </c>
       <c r="D32" t="s">
         <v>4</v>
@@ -1787,41 +2153,41 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>144</v>
+        <v>187</v>
       </c>
       <c r="C33" t="s">
-        <v>250</v>
+        <v>329</v>
       </c>
       <c r="D33" t="s">
-        <v>319</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>145</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>251</v>
+        <v>330</v>
       </c>
       <c r="D34" t="s">
-        <v>4</v>
+        <v>443</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>146</v>
+        <v>188</v>
       </c>
       <c r="C35" t="s">
-        <v>252</v>
+        <v>331</v>
       </c>
       <c r="D35" t="s">
         <v>4</v>
@@ -1829,13 +2195,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="C36" t="s">
-        <v>253</v>
+        <v>332</v>
       </c>
       <c r="D36" t="s">
         <v>4</v>
@@ -1843,13 +2209,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="C37" t="s">
-        <v>254</v>
+        <v>333</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
@@ -1857,13 +2223,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>149</v>
+        <v>191</v>
       </c>
       <c r="C38" t="s">
-        <v>255</v>
+        <v>334</v>
       </c>
       <c r="D38" t="s">
         <v>4</v>
@@ -1871,13 +2237,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>150</v>
+        <v>192</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
+        <v>335</v>
       </c>
       <c r="D39" t="s">
         <v>4</v>
@@ -1885,13 +2251,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>151</v>
+        <v>193</v>
       </c>
       <c r="C40" t="s">
-        <v>256</v>
+        <v>336</v>
       </c>
       <c r="D40" t="s">
         <v>4</v>
@@ -1899,27 +2265,27 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>152</v>
+        <v>194</v>
       </c>
       <c r="C41" t="s">
-        <v>257</v>
+        <v>337</v>
       </c>
       <c r="D41" t="s">
-        <v>319</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>153</v>
+        <v>195</v>
       </c>
       <c r="C42" t="s">
-        <v>258</v>
+        <v>338</v>
       </c>
       <c r="D42" t="s">
         <v>4</v>
@@ -1927,13 +2293,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>154</v>
+        <v>196</v>
       </c>
       <c r="C43" t="s">
-        <v>259</v>
+        <v>339</v>
       </c>
       <c r="D43" t="s">
         <v>4</v>
@@ -1941,13 +2307,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>155</v>
+        <v>197</v>
       </c>
       <c r="C44" t="s">
-        <v>260</v>
+        <v>4</v>
       </c>
       <c r="D44" t="s">
         <v>4</v>
@@ -1955,13 +2321,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>156</v>
+        <v>198</v>
       </c>
       <c r="C45" t="s">
-        <v>261</v>
+        <v>340</v>
       </c>
       <c r="D45" t="s">
         <v>4</v>
@@ -1969,13 +2335,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>157</v>
+        <v>199</v>
       </c>
       <c r="C46" t="s">
-        <v>262</v>
+        <v>341</v>
       </c>
       <c r="D46" t="s">
         <v>4</v>
@@ -1983,13 +2349,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>200</v>
       </c>
       <c r="C47" t="s">
-        <v>263</v>
+        <v>342</v>
       </c>
       <c r="D47" t="s">
         <v>4</v>
@@ -1997,41 +2363,41 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>158</v>
+        <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>4</v>
+        <v>343</v>
       </c>
       <c r="D48" t="s">
-        <v>319</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>159</v>
+        <v>201</v>
       </c>
       <c r="C49" t="s">
         <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>319</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>160</v>
+        <v>202</v>
       </c>
       <c r="C50" t="s">
-        <v>264</v>
+        <v>344</v>
       </c>
       <c r="D50" t="s">
         <v>4</v>
@@ -2039,13 +2405,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>161</v>
+        <v>203</v>
       </c>
       <c r="C51" t="s">
-        <v>265</v>
+        <v>345</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
@@ -2053,13 +2419,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>162</v>
+        <v>204</v>
       </c>
       <c r="C52" t="s">
-        <v>266</v>
+        <v>346</v>
       </c>
       <c r="D52" t="s">
         <v>4</v>
@@ -2067,27 +2433,27 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="C53" t="s">
-        <v>267</v>
+        <v>347</v>
       </c>
       <c r="D53" t="s">
-        <v>4</v>
+        <v>443</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
       <c r="C54" t="s">
-        <v>268</v>
+        <v>348</v>
       </c>
       <c r="D54" t="s">
         <v>4</v>
@@ -2095,13 +2461,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>165</v>
+        <v>207</v>
       </c>
       <c r="C55" t="s">
-        <v>269</v>
+        <v>349</v>
       </c>
       <c r="D55" t="s">
         <v>4</v>
@@ -2109,13 +2475,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>166</v>
+        <v>208</v>
       </c>
       <c r="C56" t="s">
-        <v>4</v>
+        <v>350</v>
       </c>
       <c r="D56" t="s">
         <v>4</v>
@@ -2123,13 +2489,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>167</v>
+        <v>209</v>
       </c>
       <c r="C57" t="s">
-        <v>270</v>
+        <v>351</v>
       </c>
       <c r="D57" t="s">
         <v>4</v>
@@ -2137,27 +2503,27 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="C58" t="s">
-        <v>271</v>
+        <v>352</v>
       </c>
       <c r="D58" t="s">
-        <v>319</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>169</v>
+        <v>4</v>
       </c>
       <c r="C59" t="s">
-        <v>272</v>
+        <v>353</v>
       </c>
       <c r="D59" t="s">
         <v>4</v>
@@ -2165,13 +2531,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>170</v>
+        <v>4</v>
       </c>
       <c r="C60" t="s">
-        <v>4</v>
+        <v>354</v>
       </c>
       <c r="D60" t="s">
         <v>4</v>
@@ -2179,13 +2545,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>171</v>
+        <v>211</v>
       </c>
       <c r="C61" t="s">
-        <v>273</v>
+        <v>355</v>
       </c>
       <c r="D61" t="s">
         <v>4</v>
@@ -2193,41 +2559,41 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>172</v>
+        <v>212</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
       </c>
       <c r="D62" t="s">
-        <v>319</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>173</v>
+        <v>4</v>
       </c>
       <c r="C63" t="s">
-        <v>4</v>
+        <v>356</v>
       </c>
       <c r="D63" t="s">
-        <v>319</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>174</v>
+        <v>213</v>
       </c>
       <c r="C64" t="s">
-        <v>4</v>
+        <v>357</v>
       </c>
       <c r="D64" t="s">
         <v>4</v>
@@ -2235,27 +2601,27 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>175</v>
+        <v>214</v>
       </c>
       <c r="C65" t="s">
-        <v>274</v>
+        <v>358</v>
       </c>
       <c r="D65" t="s">
-        <v>4</v>
+        <v>443</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>176</v>
+        <v>215</v>
       </c>
       <c r="C66" t="s">
-        <v>275</v>
+        <v>359</v>
       </c>
       <c r="D66" t="s">
         <v>4</v>
@@ -2263,13 +2629,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>4</v>
+        <v>216</v>
       </c>
       <c r="C67" t="s">
-        <v>276</v>
+        <v>360</v>
       </c>
       <c r="D67" t="s">
         <v>4</v>
@@ -2277,13 +2643,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>177</v>
+        <v>217</v>
       </c>
       <c r="C68" t="s">
-        <v>277</v>
+        <v>361</v>
       </c>
       <c r="D68" t="s">
         <v>4</v>
@@ -2291,13 +2657,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>178</v>
+        <v>218</v>
       </c>
       <c r="C69" t="s">
-        <v>278</v>
+        <v>362</v>
       </c>
       <c r="D69" t="s">
         <v>4</v>
@@ -2305,13 +2671,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>179</v>
+        <v>219</v>
       </c>
       <c r="C70" t="s">
-        <v>279</v>
+        <v>363</v>
       </c>
       <c r="D70" t="s">
         <v>4</v>
@@ -2319,13 +2685,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="C71" t="s">
-        <v>280</v>
+        <v>364</v>
       </c>
       <c r="D71" t="s">
         <v>4</v>
@@ -2333,13 +2699,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>181</v>
+        <v>221</v>
       </c>
       <c r="C72" t="s">
-        <v>281</v>
+        <v>365</v>
       </c>
       <c r="D72" t="s">
         <v>4</v>
@@ -2347,13 +2713,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>182</v>
+        <v>222</v>
       </c>
       <c r="C73" t="s">
-        <v>282</v>
+        <v>366</v>
       </c>
       <c r="D73" t="s">
         <v>4</v>
@@ -2361,13 +2727,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>183</v>
+        <v>4</v>
       </c>
       <c r="C74" t="s">
-        <v>283</v>
+        <v>367</v>
       </c>
       <c r="D74" t="s">
         <v>4</v>
@@ -2375,41 +2741,41 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>184</v>
+        <v>223</v>
       </c>
       <c r="C75" t="s">
-        <v>284</v>
+        <v>4</v>
       </c>
       <c r="D75" t="s">
-        <v>4</v>
+        <v>443</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>185</v>
+        <v>224</v>
       </c>
       <c r="C76" t="s">
-        <v>285</v>
+        <v>4</v>
       </c>
       <c r="D76" t="s">
-        <v>4</v>
+        <v>443</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>186</v>
+        <v>225</v>
       </c>
       <c r="C77" t="s">
-        <v>286</v>
+        <v>368</v>
       </c>
       <c r="D77" t="s">
         <v>4</v>
@@ -2417,13 +2783,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="C78" t="s">
-        <v>287</v>
+        <v>369</v>
       </c>
       <c r="D78" t="s">
         <v>4</v>
@@ -2431,13 +2797,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>188</v>
+        <v>227</v>
       </c>
       <c r="C79" t="s">
-        <v>288</v>
+        <v>370</v>
       </c>
       <c r="D79" t="s">
         <v>4</v>
@@ -2445,13 +2811,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>189</v>
+        <v>228</v>
       </c>
       <c r="C80" t="s">
-        <v>289</v>
+        <v>371</v>
       </c>
       <c r="D80" t="s">
         <v>4</v>
@@ -2459,13 +2825,13 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>190</v>
+        <v>229</v>
       </c>
       <c r="C81" t="s">
-        <v>290</v>
+        <v>372</v>
       </c>
       <c r="D81" t="s">
         <v>4</v>
@@ -2473,13 +2839,13 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>191</v>
+        <v>230</v>
       </c>
       <c r="C82" t="s">
-        <v>291</v>
+        <v>373</v>
       </c>
       <c r="D82" t="s">
         <v>4</v>
@@ -2487,13 +2853,13 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>192</v>
+        <v>231</v>
       </c>
       <c r="C83" t="s">
-        <v>85</v>
+        <v>374</v>
       </c>
       <c r="D83" t="s">
         <v>4</v>
@@ -2501,13 +2867,13 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>193</v>
+        <v>232</v>
       </c>
       <c r="C84" t="s">
-        <v>292</v>
+        <v>4</v>
       </c>
       <c r="D84" t="s">
         <v>4</v>
@@ -2515,13 +2881,13 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>194</v>
+        <v>233</v>
       </c>
       <c r="C85" t="s">
-        <v>293</v>
+        <v>375</v>
       </c>
       <c r="D85" t="s">
         <v>4</v>
@@ -2529,13 +2895,13 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>195</v>
+        <v>234</v>
       </c>
       <c r="C86" t="s">
-        <v>294</v>
+        <v>376</v>
       </c>
       <c r="D86" t="s">
         <v>4</v>
@@ -2543,27 +2909,27 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>196</v>
+        <v>235</v>
       </c>
       <c r="C87" t="s">
-        <v>295</v>
+        <v>377</v>
       </c>
       <c r="D87" t="s">
-        <v>4</v>
+        <v>443</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>197</v>
+        <v>236</v>
       </c>
       <c r="C88" t="s">
-        <v>296</v>
+        <v>378</v>
       </c>
       <c r="D88" t="s">
         <v>4</v>
@@ -2571,13 +2937,13 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>198</v>
+        <v>237</v>
       </c>
       <c r="C89" t="s">
-        <v>297</v>
+        <v>4</v>
       </c>
       <c r="D89" t="s">
         <v>4</v>
@@ -2585,13 +2951,13 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="C90" t="s">
-        <v>298</v>
+        <v>379</v>
       </c>
       <c r="D90" t="s">
         <v>4</v>
@@ -2599,41 +2965,41 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>200</v>
+        <v>239</v>
       </c>
       <c r="C91" t="s">
-        <v>299</v>
+        <v>4</v>
       </c>
       <c r="D91" t="s">
-        <v>4</v>
+        <v>443</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>201</v>
+        <v>240</v>
       </c>
       <c r="C92" t="s">
-        <v>300</v>
+        <v>4</v>
       </c>
       <c r="D92" t="s">
-        <v>4</v>
+        <v>443</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>202</v>
+        <v>241</v>
       </c>
       <c r="C93" t="s">
-        <v>301</v>
+        <v>4</v>
       </c>
       <c r="D93" t="s">
         <v>4</v>
@@ -2641,13 +3007,13 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>203</v>
+        <v>242</v>
       </c>
       <c r="C94" t="s">
-        <v>302</v>
+        <v>380</v>
       </c>
       <c r="D94" t="s">
         <v>4</v>
@@ -2655,13 +3021,13 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>204</v>
+        <v>243</v>
       </c>
       <c r="C95" t="s">
-        <v>303</v>
+        <v>381</v>
       </c>
       <c r="D95" t="s">
         <v>4</v>
@@ -2669,13 +3035,13 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="C96" t="s">
-        <v>304</v>
+        <v>382</v>
       </c>
       <c r="D96" t="s">
         <v>4</v>
@@ -2683,13 +3049,13 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>206</v>
+        <v>245</v>
       </c>
       <c r="C97" t="s">
-        <v>305</v>
+        <v>383</v>
       </c>
       <c r="D97" t="s">
         <v>4</v>
@@ -2697,13 +3063,13 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>207</v>
+        <v>246</v>
       </c>
       <c r="C98" t="s">
-        <v>306</v>
+        <v>384</v>
       </c>
       <c r="D98" t="s">
         <v>4</v>
@@ -2711,13 +3077,13 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>208</v>
+        <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>307</v>
+        <v>385</v>
       </c>
       <c r="D99" t="s">
         <v>4</v>
@@ -2725,13 +3091,13 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>209</v>
+        <v>247</v>
       </c>
       <c r="C100" t="s">
-        <v>308</v>
+        <v>386</v>
       </c>
       <c r="D100" t="s">
         <v>4</v>
@@ -2739,13 +3105,13 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>210</v>
+        <v>248</v>
       </c>
       <c r="C101" t="s">
-        <v>309</v>
+        <v>387</v>
       </c>
       <c r="D101" t="s">
         <v>4</v>
@@ -2753,13 +3119,13 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>211</v>
+        <v>249</v>
       </c>
       <c r="C102" t="s">
-        <v>4</v>
+        <v>388</v>
       </c>
       <c r="D102" t="s">
         <v>4</v>
@@ -2767,13 +3133,13 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>212</v>
+        <v>250</v>
       </c>
       <c r="C103" t="s">
-        <v>310</v>
+        <v>389</v>
       </c>
       <c r="D103" t="s">
         <v>4</v>
@@ -2781,13 +3147,13 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="C104" t="s">
-        <v>311</v>
+        <v>390</v>
       </c>
       <c r="D104" t="s">
         <v>4</v>
@@ -2795,13 +3161,13 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>214</v>
+        <v>252</v>
       </c>
       <c r="C105" t="s">
-        <v>312</v>
+        <v>391</v>
       </c>
       <c r="D105" t="s">
         <v>4</v>
@@ -2809,13 +3175,13 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>215</v>
+        <v>253</v>
       </c>
       <c r="C106" t="s">
-        <v>313</v>
+        <v>392</v>
       </c>
       <c r="D106" t="s">
         <v>4</v>
@@ -2823,13 +3189,13 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>216</v>
+        <v>254</v>
       </c>
       <c r="C107" t="s">
-        <v>314</v>
+        <v>393</v>
       </c>
       <c r="D107" t="s">
         <v>4</v>
@@ -2837,13 +3203,13 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>217</v>
+        <v>255</v>
       </c>
       <c r="C108" t="s">
-        <v>315</v>
+        <v>394</v>
       </c>
       <c r="D108" t="s">
         <v>4</v>
@@ -2851,13 +3217,13 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>218</v>
+        <v>256</v>
       </c>
       <c r="C109" t="s">
-        <v>4</v>
+        <v>395</v>
       </c>
       <c r="D109" t="s">
         <v>4</v>
@@ -2865,13 +3231,13 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>219</v>
+        <v>257</v>
       </c>
       <c r="C110" t="s">
-        <v>316</v>
+        <v>396</v>
       </c>
       <c r="D110" t="s">
         <v>4</v>
@@ -2879,13 +3245,13 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>220</v>
+        <v>258</v>
       </c>
       <c r="C111" t="s">
-        <v>317</v>
+        <v>397</v>
       </c>
       <c r="D111" t="s">
         <v>4</v>
@@ -2893,15 +3259,673 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>259</v>
+      </c>
+      <c r="C112" t="s">
+        <v>398</v>
+      </c>
+      <c r="D112" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>260</v>
+      </c>
+      <c r="C113" t="s">
+        <v>399</v>
+      </c>
+      <c r="D113" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" t="s">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>261</v>
+      </c>
+      <c r="C114" t="s">
+        <v>400</v>
+      </c>
+      <c r="D114" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" t="s">
         <v>114</v>
       </c>
-      <c r="B112" t="s">
-        <v>221</v>
-      </c>
-      <c r="C112" t="s">
-        <v>318</v>
-      </c>
-      <c r="D112" t="s">
+      <c r="B115" t="s">
+        <v>262</v>
+      </c>
+      <c r="C115" t="s">
+        <v>401</v>
+      </c>
+      <c r="D115" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" t="s">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>263</v>
+      </c>
+      <c r="C116" t="s">
+        <v>402</v>
+      </c>
+      <c r="D116" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>264</v>
+      </c>
+      <c r="C117" t="s">
+        <v>403</v>
+      </c>
+      <c r="D117" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="s">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>265</v>
+      </c>
+      <c r="C118" t="s">
+        <v>404</v>
+      </c>
+      <c r="D118" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" t="s">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>266</v>
+      </c>
+      <c r="C119" t="s">
+        <v>405</v>
+      </c>
+      <c r="D119" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" t="s">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>267</v>
+      </c>
+      <c r="C120" t="s">
+        <v>406</v>
+      </c>
+      <c r="D120" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>268</v>
+      </c>
+      <c r="C121" t="s">
+        <v>120</v>
+      </c>
+      <c r="D121" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" t="s">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>269</v>
+      </c>
+      <c r="C122" t="s">
+        <v>407</v>
+      </c>
+      <c r="D122" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" t="s">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>270</v>
+      </c>
+      <c r="C123" t="s">
+        <v>408</v>
+      </c>
+      <c r="D123" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" t="s">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>271</v>
+      </c>
+      <c r="C124" t="s">
+        <v>409</v>
+      </c>
+      <c r="D124" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" t="s">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>272</v>
+      </c>
+      <c r="C125" t="s">
+        <v>410</v>
+      </c>
+      <c r="D125" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" t="s">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>273</v>
+      </c>
+      <c r="C126" t="s">
+        <v>411</v>
+      </c>
+      <c r="D126" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" t="s">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>274</v>
+      </c>
+      <c r="C127" t="s">
+        <v>412</v>
+      </c>
+      <c r="D127" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" t="s">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>275</v>
+      </c>
+      <c r="C128" t="s">
+        <v>413</v>
+      </c>
+      <c r="D128" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" t="s">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>276</v>
+      </c>
+      <c r="C129" t="s">
+        <v>414</v>
+      </c>
+      <c r="D129" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" t="s">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>277</v>
+      </c>
+      <c r="C130" t="s">
+        <v>415</v>
+      </c>
+      <c r="D130" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" t="s">
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
+        <v>278</v>
+      </c>
+      <c r="C131" t="s">
+        <v>416</v>
+      </c>
+      <c r="D131" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" t="s">
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
+        <v>279</v>
+      </c>
+      <c r="C132" t="s">
+        <v>417</v>
+      </c>
+      <c r="D132" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" t="s">
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
+        <v>280</v>
+      </c>
+      <c r="C133" t="s">
+        <v>418</v>
+      </c>
+      <c r="D133" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" t="s">
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
+        <v>281</v>
+      </c>
+      <c r="C134" t="s">
+        <v>419</v>
+      </c>
+      <c r="D134" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" t="s">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>282</v>
+      </c>
+      <c r="C135" t="s">
+        <v>420</v>
+      </c>
+      <c r="D135" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" t="s">
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
+        <v>283</v>
+      </c>
+      <c r="C136" t="s">
+        <v>421</v>
+      </c>
+      <c r="D136" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" t="s">
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
+        <v>284</v>
+      </c>
+      <c r="C137" t="s">
+        <v>422</v>
+      </c>
+      <c r="D137" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" t="s">
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
+        <v>285</v>
+      </c>
+      <c r="C138" t="s">
+        <v>423</v>
+      </c>
+      <c r="D138" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" t="s">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>286</v>
+      </c>
+      <c r="C139" t="s">
+        <v>424</v>
+      </c>
+      <c r="D139" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" t="s">
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
+        <v>287</v>
+      </c>
+      <c r="C140" t="s">
+        <v>4</v>
+      </c>
+      <c r="D140" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" t="s">
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
+        <v>288</v>
+      </c>
+      <c r="C141" t="s">
+        <v>425</v>
+      </c>
+      <c r="D141" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" t="s">
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
+        <v>289</v>
+      </c>
+      <c r="C142" t="s">
+        <v>426</v>
+      </c>
+      <c r="D142" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" t="s">
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
+        <v>290</v>
+      </c>
+      <c r="C143" t="s">
+        <v>427</v>
+      </c>
+      <c r="D143" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" t="s">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>291</v>
+      </c>
+      <c r="C144" t="s">
+        <v>428</v>
+      </c>
+      <c r="D144" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" t="s">
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
+        <v>292</v>
+      </c>
+      <c r="C145" t="s">
+        <v>429</v>
+      </c>
+      <c r="D145" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" t="s">
+        <v>145</v>
+      </c>
+      <c r="B146" t="s">
+        <v>293</v>
+      </c>
+      <c r="C146" t="s">
+        <v>430</v>
+      </c>
+      <c r="D146" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" t="s">
+        <v>146</v>
+      </c>
+      <c r="B147" t="s">
+        <v>294</v>
+      </c>
+      <c r="C147" t="s">
+        <v>431</v>
+      </c>
+      <c r="D147" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" t="s">
+        <v>147</v>
+      </c>
+      <c r="B148" t="s">
+        <v>295</v>
+      </c>
+      <c r="C148" t="s">
+        <v>4</v>
+      </c>
+      <c r="D148" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" t="s">
+        <v>148</v>
+      </c>
+      <c r="B149" t="s">
+        <v>296</v>
+      </c>
+      <c r="C149" t="s">
+        <v>432</v>
+      </c>
+      <c r="D149" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" t="s">
+        <v>149</v>
+      </c>
+      <c r="B150" t="s">
+        <v>297</v>
+      </c>
+      <c r="C150" t="s">
+        <v>433</v>
+      </c>
+      <c r="D150" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" t="s">
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
+        <v>298</v>
+      </c>
+      <c r="C151" t="s">
+        <v>434</v>
+      </c>
+      <c r="D151" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" t="s">
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
+        <v>299</v>
+      </c>
+      <c r="C152" t="s">
+        <v>435</v>
+      </c>
+      <c r="D152" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" t="s">
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
+        <v>300</v>
+      </c>
+      <c r="C153" t="s">
+        <v>436</v>
+      </c>
+      <c r="D153" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" t="s">
+        <v>153</v>
+      </c>
+      <c r="B154" t="s">
+        <v>301</v>
+      </c>
+      <c r="C154" t="s">
+        <v>437</v>
+      </c>
+      <c r="D154" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" t="s">
+        <v>154</v>
+      </c>
+      <c r="B155" t="s">
+        <v>302</v>
+      </c>
+      <c r="C155" t="s">
+        <v>438</v>
+      </c>
+      <c r="D155" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" t="s">
+        <v>155</v>
+      </c>
+      <c r="B156" t="s">
+        <v>303</v>
+      </c>
+      <c r="C156" t="s">
+        <v>439</v>
+      </c>
+      <c r="D156" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" t="s">
+        <v>156</v>
+      </c>
+      <c r="B157" t="s">
+        <v>304</v>
+      </c>
+      <c r="C157" t="s">
+        <v>440</v>
+      </c>
+      <c r="D157" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" t="s">
+        <v>157</v>
+      </c>
+      <c r="B158" t="s">
+        <v>305</v>
+      </c>
+      <c r="C158" t="s">
+        <v>441</v>
+      </c>
+      <c r="D158" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" t="s">
+        <v>158</v>
+      </c>
+      <c r="B159" t="s">
+        <v>306</v>
+      </c>
+      <c r="C159" t="s">
+        <v>442</v>
+      </c>
+      <c r="D159" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>